<commit_message>
dopest night of coding ever. pie chart is at basic completeness.
</commit_message>
<xml_diff>
--- a/climbers-partial.xlsx
+++ b/climbers-partial.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="19200" windowHeight="7638"/>
+    <workbookView xWindow="0" yWindow="912" windowWidth="19200" windowHeight="7638"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>